<commit_message>
Add Reporting html and Gmail Email integration
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel/TestDataSheet.xlsx
+++ b/src/main/resources/Excel/TestDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdafsarali/Downloads/KeywordDrivenFramework/src/main/resources/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1FDFF2-98D6-6947-B60C-41EF830E1639}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E8DD8-87A0-A344-BB45-85BA6051A530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="66">
   <si>
     <t>SuiteName</t>
   </si>
@@ -206,6 +206,21 @@
   </si>
   <si>
     <t>Simple Login Details</t>
+  </si>
+  <si>
+    <t>Simple Login Details 2</t>
+  </si>
+  <si>
+    <t>Simple Login Details 3</t>
+  </si>
+  <si>
+    <t>Simple Login Details 4</t>
+  </si>
+  <si>
+    <t>Simple Login Details 5</t>
+  </si>
+  <si>
+    <t>Simple Login Details 6</t>
   </si>
 </sst>
 </file>
@@ -639,7 +654,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -851,7 +866,7 @@
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1029,7 +1044,7 @@
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1207,7 +1222,7 @@
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1385,7 +1400,7 @@
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -1563,7 +1578,7 @@
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8"/>
       <c r="B52" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1749,6 +1764,7 @@
     <hyperlink ref="F57" r:id="rId6" display="Test@123" xr:uid="{51009542-A76E-EA45-AE04-B20D11AF8A74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update and refactor classes
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel/TestDataSheet.xlsx
+++ b/src/main/resources/Excel/TestDataSheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdafsarali/Downloads/KeywordDrivenFramework/src/main/resources/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E8DD8-87A0-A344-BB45-85BA6051A530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E85026-EBC7-6241-899F-2B7081CB94D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
-    <sheet name="SuiteDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSteps" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="71">
   <si>
     <t>SuiteName</t>
   </si>
@@ -55,9 +55,6 @@
     <t>LogIn_01</t>
   </si>
   <si>
-    <t>Login with Valid username and password</t>
-  </si>
-  <si>
     <t>TestId</t>
   </si>
   <si>
@@ -221,6 +218,24 @@
   </si>
   <si>
     <t>Simple Login Details 6</t>
+  </si>
+  <si>
+    <t>Simple Login Details1</t>
+  </si>
+  <si>
+    <t>Simple Login Details2</t>
+  </si>
+  <si>
+    <t>Simple Login Details3</t>
+  </si>
+  <si>
+    <t>Simple Login Details4</t>
+  </si>
+  <si>
+    <t>Simple Login Details5</t>
+  </si>
+  <si>
+    <t>Simple Login Details6</t>
   </si>
 </sst>
 </file>
@@ -329,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -343,6 +358,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +627,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -638,10 +654,66 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -653,8 +725,8 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView zoomScale="143" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -664,31 +736,31 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -701,15 +773,15 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -718,15 +790,15 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -735,16 +807,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -754,19 +826,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -775,19 +847,19 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -796,16 +868,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -815,12 +887,12 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
@@ -832,16 +904,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -851,14 +923,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -866,7 +938,7 @@
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -876,129 +948,129 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="4">
         <v>5</v>
@@ -1007,36 +1079,36 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1044,7 +1116,7 @@
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1054,129 +1126,129 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="4">
         <v>5</v>
@@ -1185,36 +1257,36 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1222,7 +1294,7 @@
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1232,129 +1304,129 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="4">
         <v>5</v>
@@ -1363,36 +1435,36 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1400,7 +1472,7 @@
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -1410,129 +1482,129 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E45" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F49" s="4">
         <v>5</v>
@@ -1541,36 +1613,36 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1578,7 +1650,7 @@
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8"/>
       <c r="B52" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1588,129 +1660,129 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E55" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F59" s="4">
         <v>5</v>
@@ -1719,36 +1791,36 @@
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D60" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -1781,54 +1853,54 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1836,7 +1908,7 @@
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1844,7 +1916,7 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1852,7 +1924,7 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>